<commit_message>
update a bug in GMIT93 test
</commit_message>
<xml_diff>
--- a/scoring/tests/GMIT/GMIT93_test_1.xlsx
+++ b/scoring/tests/GMIT/GMIT93_test_1.xlsx
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
add new GMIT93 tests
</commit_message>
<xml_diff>
--- a/scoring/tests/GMIT/GMIT93_test_1.xlsx
+++ b/scoring/tests/GMIT/GMIT93_test_1.xlsx
@@ -440,7 +440,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>